<commit_message>
Everything works, needs some tuning
</commit_message>
<xml_diff>
--- a/output-files/Div-3.xlsx
+++ b/output-files/Div-3.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
-  <si>
-    <t>RANK</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+  <si>
+    <t>COLLEGE-RANK</t>
+  </si>
+  <si>
+    <t>CONTEST-RANK</t>
   </si>
   <si>
     <t>USER-NAME</t>
@@ -25,79 +28,109 @@
     <t>SCORE</t>
   </si>
   <si>
-    <t>775</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>242</t>
+  </si>
+  <si>
+    <t>jai_21r01a7238</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1286</t>
+  </si>
+  <si>
+    <t>abhinay2001</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2064</t>
+  </si>
+  <si>
+    <t>shiva7ganesh</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2347</t>
+  </si>
+  <si>
+    <t>vyshnavi6764</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2485</t>
+  </si>
+  <si>
+    <t>praneeth702</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>2830</t>
+  </si>
+  <si>
+    <t>swarna_569</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>abhiram_2023</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>2836</t>
   </si>
   <si>
     <t>saibharath502</t>
   </si>
   <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>1018</t>
-  </si>
-  <si>
-    <t>jai_21r01a7238</t>
-  </si>
-  <si>
-    <t>2245</t>
-  </si>
-  <si>
-    <t>narendra3</t>
-  </si>
-  <si>
-    <t>2447</t>
-  </si>
-  <si>
-    <t>shradha_317</t>
-  </si>
-  <si>
-    <t>2466</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>3311</t>
   </si>
   <si>
     <t>dileep1111</t>
   </si>
   <si>
-    <t>3077</t>
-  </si>
-  <si>
-    <t>shiva7ganesh</t>
-  </si>
-  <si>
-    <t>3223</t>
-  </si>
-  <si>
-    <t>praneeth702</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>3253</t>
-  </si>
-  <si>
-    <t>sk50412</t>
-  </si>
-  <si>
-    <t>3301</t>
-  </si>
-  <si>
-    <t>vinay_vinay</t>
-  </si>
-  <si>
-    <t>3329</t>
-  </si>
-  <si>
-    <t>bhanu250602</t>
-  </si>
-  <si>
-    <t>3491</t>
+    <t>100</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>3341</t>
   </si>
   <si>
     <t>varshitha_77</t>
   </si>
   <si>
-    <t>100</t>
+    <t>11</t>
+  </si>
+  <si>
+    <t>3421</t>
+  </si>
+  <si>
+    <t>saipriya2003</t>
   </si>
 </sst>
 </file>
@@ -429,13 +462,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,247 +478,162 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" t="s">
-        <v>27</v>
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>